<commit_message>
fix(envClass_csv): fix data semantics
</commit_message>
<xml_diff>
--- a/DSMCaseReasoning/src/envClass.xlsx
+++ b/DSMCaseReasoning/src/envClass.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F9632F-83EC-4F1F-93A2-E9A12BA3894A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90198E0-EB49-4F41-A20D-C5D81BE91876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="446">
   <si>
     <t>Altitude above channel network</t>
   </si>
@@ -1681,12 +1681,44 @@
     <t>RPI</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>dem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>convergence_index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>profile_curvature</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plan_curvature</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>slope</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>flow_direction</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>topographic_wetness_index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stream_power_index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2121,16 +2153,16 @@
       <selection activeCell="A2" sqref="A2:A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="79.44140625" customWidth="1"/>
+    <col min="5" max="5" width="79.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>335</v>
       </c>
@@ -2147,7 +2179,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="41.4">
+    <row r="2" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -2161,27 +2193,27 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>113</v>
       </c>
@@ -2189,17 +2221,17 @@
         <v>281</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>188</v>
       </c>
@@ -2210,7 +2242,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="69">
+    <row r="11" spans="1:5" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>190</v>
       </c>
@@ -2221,7 +2253,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="41.4">
+    <row r="12" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>202</v>
       </c>
@@ -2235,7 +2267,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>246</v>
       </c>
@@ -2243,7 +2275,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="27.6">
+    <row r="14" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>252</v>
       </c>
@@ -2251,12 +2283,12 @@
         <v>253</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>271</v>
       </c>
@@ -2278,15 +2310,15 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="65.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.6640625" customWidth="1"/>
+    <col min="1" max="1" width="65.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>335</v>
       </c>
@@ -2303,7 +2335,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>282</v>
       </c>
@@ -2311,7 +2343,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>283</v>
       </c>
@@ -2319,17 +2351,17 @@
         <v>221</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>286</v>
       </c>
@@ -2337,12 +2369,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>288</v>
       </c>
@@ -2350,7 +2382,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>289</v>
       </c>
@@ -2361,7 +2393,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="41.4">
+    <row r="10" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>290</v>
       </c>
@@ -2372,7 +2404,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="27.6">
+    <row r="11" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>291</v>
       </c>
@@ -2383,32 +2415,32 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="41.4">
+    <row r="17" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>297</v>
       </c>
@@ -2416,7 +2448,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="41.4">
+    <row r="18" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>298</v>
       </c>
@@ -2424,7 +2456,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="41.4">
+    <row r="19" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>299</v>
       </c>
@@ -2432,7 +2464,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="41.4">
+    <row r="20" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>300</v>
       </c>
@@ -2440,27 +2472,27 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -2468,7 +2500,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>305</v>
       </c>
@@ -2476,7 +2508,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>306</v>
       </c>
@@ -2484,7 +2516,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="41.4">
+    <row r="28" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>307</v>
       </c>
@@ -2492,7 +2524,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>308</v>
       </c>
@@ -2500,7 +2532,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="41.4">
+    <row r="30" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>309</v>
       </c>
@@ -2508,7 +2540,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="41.4">
+    <row r="31" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>310</v>
       </c>
@@ -2516,7 +2548,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>311</v>
       </c>
@@ -2524,7 +2556,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="41.4">
+    <row r="33" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>312</v>
       </c>
@@ -2532,7 +2564,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="41.4">
+    <row r="34" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>313</v>
       </c>
@@ -2540,7 +2572,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="41.4">
+    <row r="35" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>314</v>
       </c>
@@ -2548,7 +2580,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="138">
+    <row r="36" spans="1:5" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>315</v>
       </c>
@@ -2556,7 +2588,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>316</v>
       </c>
@@ -2564,7 +2596,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>317</v>
       </c>
@@ -2572,7 +2604,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>318</v>
       </c>
@@ -2580,7 +2612,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>319</v>
       </c>
@@ -2588,7 +2620,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>320</v>
       </c>
@@ -2596,7 +2628,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="82.8">
+    <row r="42" spans="1:5" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>321</v>
       </c>
@@ -2607,7 +2639,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="55.2">
+    <row r="43" spans="1:5" ht="57" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>322</v>
       </c>
@@ -2615,7 +2647,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>189</v>
       </c>
@@ -2623,7 +2655,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>323</v>
       </c>
@@ -2631,7 +2663,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="41.4">
+    <row r="46" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>205</v>
       </c>
@@ -2642,7 +2674,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>324</v>
       </c>
@@ -2653,7 +2685,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>270</v>
       </c>
@@ -2679,16 +2711,16 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.44140625" customWidth="1"/>
+    <col min="1" max="1" width="41.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.77734375" customWidth="1"/>
+    <col min="5" max="5" width="53.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>335</v>
       </c>
@@ -2705,7 +2737,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -2713,7 +2745,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -2724,7 +2756,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -2732,7 +2764,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -2740,7 +2772,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -2748,7 +2780,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -2756,7 +2788,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -2764,7 +2796,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>58</v>
       </c>
@@ -2772,7 +2804,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>59</v>
       </c>
@@ -2780,7 +2812,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -2788,7 +2820,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>62</v>
       </c>
@@ -2796,7 +2828,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>63</v>
       </c>
@@ -2804,7 +2836,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -2812,12 +2844,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -2831,7 +2863,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>102</v>
       </c>
@@ -2842,17 +2874,17 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -2860,7 +2892,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>70</v>
       </c>
@@ -2868,7 +2900,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>71</v>
       </c>
@@ -2879,7 +2911,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>72</v>
       </c>
@@ -2887,17 +2919,17 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>78</v>
       </c>
@@ -2908,7 +2940,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>79</v>
       </c>
@@ -2919,7 +2951,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>80</v>
       </c>
@@ -2927,17 +2959,17 @@
         <v>190</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>108</v>
       </c>
@@ -2945,22 +2977,22 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>96</v>
       </c>
@@ -2968,42 +3000,42 @@
         <v>165</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="27.6">
+    <row r="43" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>210</v>
       </c>
@@ -3014,7 +3046,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="55.2">
+    <row r="44" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>214</v>
       </c>
@@ -3028,7 +3060,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>237</v>
       </c>
@@ -3039,7 +3071,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>244</v>
       </c>
@@ -3047,7 +3079,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="69">
+    <row r="47" spans="1:5" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>266</v>
       </c>
@@ -3058,7 +3090,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>268</v>
       </c>
@@ -3066,7 +3098,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>269</v>
       </c>
@@ -3088,17 +3120,17 @@
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.33203125" customWidth="1"/>
-    <col min="4" max="4" width="39.44140625" customWidth="1"/>
-    <col min="5" max="5" width="52.109375" customWidth="1"/>
-    <col min="6" max="6" width="40.109375" customWidth="1"/>
+    <col min="3" max="3" width="61.375" customWidth="1"/>
+    <col min="4" max="4" width="39.5" customWidth="1"/>
+    <col min="5" max="5" width="52.125" customWidth="1"/>
+    <col min="6" max="6" width="40.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>335</v>
       </c>
@@ -3115,7 +3147,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -3126,7 +3158,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="41.4">
+    <row r="3" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3143,7 +3175,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>186</v>
       </c>
@@ -3151,7 +3183,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
@@ -3165,7 +3197,7 @@
         <v>39179</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>248</v>
       </c>
@@ -3174,7 +3206,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>184</v>
       </c>
@@ -3183,7 +3215,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="69">
+    <row r="8" spans="1:5" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>19</v>
       </c>
@@ -3200,7 +3232,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
@@ -3212,7 +3244,7 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" ht="55.2">
+    <row r="10" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
         <v>29</v>
       </c>
@@ -3229,7 +3261,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
         <v>173</v>
       </c>
@@ -3240,7 +3272,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>17</v>
       </c>
@@ -3248,7 +3280,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>0</v>
       </c>
@@ -3259,7 +3291,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
         <v>22</v>
       </c>
@@ -3270,7 +3302,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>26</v>
       </c>
@@ -3281,7 +3313,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
         <v>129</v>
       </c>
@@ -3289,7 +3321,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="55.2">
+    <row r="17" spans="1:5" ht="57" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>137</v>
       </c>
@@ -3300,7 +3332,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
         <v>149</v>
       </c>
@@ -3308,7 +3340,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
         <v>147</v>
       </c>
@@ -3316,7 +3348,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="27.6">
+    <row r="20" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>148</v>
       </c>
@@ -3327,7 +3359,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
         <v>328</v>
       </c>
@@ -3335,7 +3367,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>150</v>
       </c>
@@ -3343,7 +3375,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
         <v>151</v>
       </c>
@@ -3351,7 +3383,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>236</v>
       </c>
@@ -3359,7 +3391,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>152</v>
       </c>
@@ -3370,7 +3402,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
         <v>6</v>
       </c>
@@ -3381,17 +3413,17 @@
         <v>244</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="41.4">
+    <row r="29" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>349</v>
       </c>
@@ -3408,7 +3440,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>14</v>
       </c>
@@ -3419,7 +3451,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>153</v>
       </c>
@@ -3427,7 +3459,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
         <v>154</v>
       </c>
@@ -3435,7 +3467,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>155</v>
       </c>
@@ -3446,7 +3478,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="41.4">
+    <row r="34" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>156</v>
       </c>
@@ -3460,7 +3492,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="55.2">
+    <row r="35" spans="1:5" ht="57" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
         <v>124</v>
       </c>
@@ -3474,7 +3506,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
         <v>157</v>
       </c>
@@ -3482,7 +3514,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="69">
+    <row r="37" spans="1:5" ht="57" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="s">
         <v>158</v>
       </c>
@@ -3496,12 +3528,12 @@
         <v>242</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="13" t="s">
         <v>33</v>
       </c>
@@ -3509,7 +3541,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="13" t="s">
         <v>34</v>
       </c>
@@ -3517,7 +3549,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="27.6">
+    <row r="41" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A41" s="13" t="s">
         <v>119</v>
       </c>
@@ -3528,12 +3560,12 @@
         <v>155</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="14" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="16" t="s">
         <v>160</v>
       </c>
@@ -3541,12 +3573,12 @@
         <v>127</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="16" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="16" t="s">
         <v>159</v>
       </c>
@@ -3554,7 +3586,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="151.80000000000001">
+    <row r="46" spans="1:5" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A46" s="16" t="s">
         <v>180</v>
       </c>
@@ -3566,7 +3598,7 @@
         <v>241186244</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="55.2">
+    <row r="47" spans="1:5" ht="57" x14ac:dyDescent="0.2">
       <c r="A47" s="16" t="s">
         <v>135</v>
       </c>
@@ -3578,7 +3610,7 @@
         <v>117186</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="55.2">
+    <row r="48" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A48" s="16" t="s">
         <v>181</v>
       </c>
@@ -3590,7 +3622,7 @@
         <v>186244</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="16" t="s">
         <v>144</v>
       </c>
@@ -3601,7 +3633,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="16" t="s">
         <v>182</v>
       </c>
@@ -3609,7 +3641,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>183</v>
       </c>
@@ -3620,7 +3652,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="41.4">
+    <row r="52" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>167</v>
       </c>
@@ -3637,7 +3669,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="4" customFormat="1">
+    <row r="53" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>330</v>
       </c>
@@ -3645,7 +3677,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="124.2">
+    <row r="54" spans="1:5" ht="114" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>331</v>
       </c>
@@ -3656,7 +3688,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="17" t="s">
         <v>208</v>
       </c>
@@ -3664,7 +3696,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="17" t="s">
         <v>209</v>
       </c>
@@ -3672,12 +3704,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="17" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="17" t="s">
         <v>193</v>
       </c>
@@ -3685,7 +3717,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="55.2">
+    <row r="59" spans="1:5" ht="57" x14ac:dyDescent="0.2">
       <c r="A59" s="17" t="s">
         <v>194</v>
       </c>
@@ -3699,7 +3731,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="55.2">
+    <row r="60" spans="1:5" ht="57" x14ac:dyDescent="0.2">
       <c r="A60" s="17" t="s">
         <v>195</v>
       </c>
@@ -3710,7 +3742,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="27.6">
+    <row r="61" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>217</v>
       </c>
@@ -3721,7 +3753,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>226</v>
       </c>
@@ -3735,7 +3767,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>239</v>
       </c>
@@ -3743,7 +3775,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="82.8">
+    <row r="64" spans="1:5" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>240</v>
       </c>
@@ -3754,7 +3786,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
         <v>245</v>
       </c>
@@ -3762,7 +3794,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="55.2">
+    <row r="66" spans="1:5" ht="57" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>232</v>
       </c>
@@ -3776,7 +3808,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>254</v>
       </c>
@@ -3784,7 +3816,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>255</v>
       </c>
@@ -3792,7 +3824,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="27.6">
+    <row r="69" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A69" s="20" t="s">
         <v>256</v>
       </c>
@@ -3803,13 +3835,13 @@
         <v>257</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="20" t="s">
         <v>264</v>
       </c>
       <c r="C70" s="2"/>
     </row>
-    <row r="71" spans="1:5" ht="27.6">
+    <row r="71" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A71" s="20" t="s">
         <v>258</v>
       </c>
@@ -3817,7 +3849,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="41.4">
+    <row r="72" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>272</v>
       </c>
@@ -3828,7 +3860,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>276</v>
       </c>
@@ -3836,7 +3868,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>348</v>
       </c>
@@ -3844,7 +3876,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="9" t="s">
         <v>130</v>
       </c>
@@ -3852,7 +3884,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="9" t="s">
         <v>131</v>
       </c>
@@ -3860,7 +3892,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="9" t="s">
         <v>132</v>
       </c>
@@ -3868,7 +3900,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="9" t="s">
         <v>247</v>
       </c>
@@ -3877,7 +3909,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>179</v>
       </c>
@@ -3885,7 +3917,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>141</v>
       </c>
@@ -3899,7 +3931,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="55.2">
+    <row r="81" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A81" s="10" t="s">
         <v>121</v>
       </c>
@@ -3913,12 +3945,12 @@
         <v>155</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="9" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="15" t="s">
         <v>1</v>
       </c>
@@ -3929,12 +3961,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="19" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="27.6">
+    <row r="85" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A85" s="19" t="s">
         <v>222</v>
       </c>
@@ -3945,7 +3977,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="19" t="s">
         <v>228</v>
       </c>
@@ -3953,7 +3985,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="11" t="s">
         <v>263</v>
       </c>
@@ -3961,12 +3993,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="11" t="s">
         <v>333</v>
       </c>
@@ -3977,7 +4009,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="11" t="s">
         <v>279</v>
       </c>
@@ -3985,7 +4017,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="11" t="s">
         <v>280</v>
       </c>
@@ -3993,7 +4025,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="27.6">
+    <row r="92" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>274</v>
       </c>
@@ -4004,7 +4036,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="27.6">
+    <row r="93" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>277</v>
       </c>
@@ -4029,14 +4061,14 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="67.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="59.109375" customWidth="1"/>
+    <col min="1" max="1" width="67.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="59.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>335</v>
       </c>
@@ -4053,17 +4085,17 @@
         <v>339</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="69">
+    <row r="4" spans="1:5" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>161</v>
       </c>
@@ -4077,7 +4109,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="27.6">
+    <row r="5" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>93</v>
       </c>
@@ -4085,7 +4117,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="27.6">
+    <row r="6" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>351</v>
       </c>
@@ -4093,7 +4125,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="27.6">
+    <row r="7" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>94</v>
       </c>
@@ -4101,7 +4133,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="27.6">
+    <row r="8" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>95</v>
       </c>
@@ -4109,7 +4141,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="27.6">
+    <row r="9" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>350</v>
       </c>
@@ -4117,7 +4149,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="27.6">
+    <row r="10" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>91</v>
       </c>
@@ -4125,7 +4157,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="27.6">
+    <row r="11" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>86</v>
       </c>
@@ -4133,7 +4165,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>199</v>
       </c>
@@ -4141,12 +4173,12 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="124.2">
+    <row r="14" spans="1:5" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>249</v>
       </c>
@@ -4160,7 +4192,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>243</v>
       </c>
@@ -4182,14 +4214,14 @@
       <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>335</v>
       </c>
@@ -4206,7 +4238,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>75</v>
       </c>
@@ -4214,7 +4246,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>76</v>
       </c>
@@ -4222,7 +4254,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>77</v>
       </c>
@@ -4240,18 +4272,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5475894C-0183-485C-A84F-C14E44221D4E}">
   <dimension ref="A1:E160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="E142" sqref="E142"/>
+    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="H134" sqref="H134"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="65.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>388</v>
       </c>
@@ -4262,7 +4294,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -4273,7 +4305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>103</v>
       </c>
@@ -4284,7 +4316,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>111</v>
       </c>
@@ -4295,7 +4327,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>112</v>
       </c>
@@ -4306,7 +4338,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -4317,7 +4349,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>114</v>
       </c>
@@ -4328,7 +4360,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>185</v>
       </c>
@@ -4339,7 +4371,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>188</v>
       </c>
@@ -4350,7 +4382,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>190</v>
       </c>
@@ -4361,7 +4393,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>202</v>
       </c>
@@ -4372,7 +4404,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>246</v>
       </c>
@@ -4383,7 +4415,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>252</v>
       </c>
@@ -4394,7 +4426,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>363</v>
       </c>
@@ -4405,7 +4437,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>271</v>
       </c>
@@ -4416,7 +4448,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>282</v>
       </c>
@@ -4427,7 +4459,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>283</v>
       </c>
@@ -4438,7 +4470,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>284</v>
       </c>
@@ -4449,7 +4481,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>285</v>
       </c>
@@ -4460,7 +4492,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>286</v>
       </c>
@@ -4471,7 +4503,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>287</v>
       </c>
@@ -4482,7 +4514,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>288</v>
       </c>
@@ -4493,7 +4525,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>324</v>
       </c>
@@ -4504,7 +4536,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>290</v>
       </c>
@@ -4515,7 +4547,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>291</v>
       </c>
@@ -4526,7 +4558,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>292</v>
       </c>
@@ -4537,7 +4569,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>294</v>
       </c>
@@ -4548,7 +4580,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>295</v>
       </c>
@@ -4559,7 +4591,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>296</v>
       </c>
@@ -4570,7 +4602,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>297</v>
       </c>
@@ -4581,7 +4613,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>298</v>
       </c>
@@ -4592,7 +4624,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>299</v>
       </c>
@@ -4603,7 +4635,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>300</v>
       </c>
@@ -4614,7 +4646,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>301</v>
       </c>
@@ -4625,7 +4657,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -4636,7 +4668,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>305</v>
       </c>
@@ -4647,7 +4679,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>306</v>
       </c>
@@ -4658,7 +4690,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>307</v>
       </c>
@@ -4669,7 +4701,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>308</v>
       </c>
@@ -4680,7 +4712,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>309</v>
       </c>
@@ -4691,7 +4723,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>310</v>
       </c>
@@ -4702,7 +4734,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>311</v>
       </c>
@@ -4713,7 +4745,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>312</v>
       </c>
@@ -4724,7 +4756,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>313</v>
       </c>
@@ -4735,7 +4767,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>314</v>
       </c>
@@ -4746,7 +4778,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>315</v>
       </c>
@@ -4757,7 +4789,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>362</v>
       </c>
@@ -4768,7 +4800,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>317</v>
       </c>
@@ -4779,7 +4811,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>318</v>
       </c>
@@ -4790,7 +4822,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>319</v>
       </c>
@@ -4801,7 +4833,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>320</v>
       </c>
@@ -4812,7 +4844,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>321</v>
       </c>
@@ -4823,7 +4855,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>322</v>
       </c>
@@ -4834,7 +4866,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>189</v>
       </c>
@@ -4845,7 +4877,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>323</v>
       </c>
@@ -4856,7 +4888,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>205</v>
       </c>
@@ -4867,7 +4899,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>255</v>
       </c>
@@ -4878,7 +4910,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>357</v>
       </c>
@@ -4889,7 +4921,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>151</v>
       </c>
@@ -4900,7 +4932,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>52</v>
       </c>
@@ -4911,7 +4943,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>53</v>
       </c>
@@ -4922,7 +4954,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>54</v>
       </c>
@@ -4933,7 +4965,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>55</v>
       </c>
@@ -4944,7 +4976,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>56</v>
       </c>
@@ -4955,7 +4987,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>57</v>
       </c>
@@ -4966,7 +4998,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>58</v>
       </c>
@@ -4977,7 +5009,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>59</v>
       </c>
@@ -4988,7 +5020,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>61</v>
       </c>
@@ -4999,7 +5031,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>62</v>
       </c>
@@ -5010,7 +5042,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>63</v>
       </c>
@@ -5021,7 +5053,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>64</v>
       </c>
@@ -5032,7 +5064,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>65</v>
       </c>
@@ -5043,7 +5075,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>66</v>
       </c>
@@ -5054,7 +5086,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>102</v>
       </c>
@@ -5065,7 +5097,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>67</v>
       </c>
@@ -5076,7 +5108,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>68</v>
       </c>
@@ -5087,7 +5119,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>69</v>
       </c>
@@ -5098,7 +5130,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>70</v>
       </c>
@@ -5109,7 +5141,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>71</v>
       </c>
@@ -5120,7 +5152,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>72</v>
       </c>
@@ -5131,7 +5163,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>73</v>
       </c>
@@ -5142,7 +5174,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>74</v>
       </c>
@@ -5153,7 +5185,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>78</v>
       </c>
@@ -5164,7 +5196,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>79</v>
       </c>
@@ -5175,7 +5207,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>80</v>
       </c>
@@ -5186,7 +5218,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>365</v>
       </c>
@@ -5197,7 +5229,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>87</v>
       </c>
@@ -5208,7 +5240,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>108</v>
       </c>
@@ -5219,7 +5251,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>92</v>
       </c>
@@ -5230,7 +5262,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>96</v>
       </c>
@@ -5241,7 +5273,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>327</v>
       </c>
@@ -5252,7 +5284,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>105</v>
       </c>
@@ -5263,7 +5295,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>106</v>
       </c>
@@ -5274,7 +5306,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>326</v>
       </c>
@@ -5285,7 +5317,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>364</v>
       </c>
@@ -5296,7 +5328,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>116</v>
       </c>
@@ -5307,7 +5339,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>109</v>
       </c>
@@ -5318,7 +5350,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>210</v>
       </c>
@@ -5329,7 +5361,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>214</v>
       </c>
@@ -5340,7 +5372,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>237</v>
       </c>
@@ -5351,7 +5383,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>244</v>
       </c>
@@ -5362,7 +5394,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>266</v>
       </c>
@@ -5373,7 +5405,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>268</v>
       </c>
@@ -5384,7 +5416,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>269</v>
       </c>
@@ -5395,7 +5427,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>368</v>
       </c>
@@ -5406,9 +5438,9 @@
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>19</v>
+        <v>444</v>
       </c>
       <c r="B106" t="s">
         <v>345</v>
@@ -5417,7 +5449,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>29</v>
       </c>
@@ -5428,7 +5460,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>173</v>
       </c>
@@ -5439,7 +5471,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>355</v>
       </c>
@@ -5450,7 +5482,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>356</v>
       </c>
@@ -5461,9 +5493,9 @@
         <v>111</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>137</v>
+        <v>443</v>
       </c>
       <c r="B111" t="s">
         <v>345</v>
@@ -5472,7 +5504,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>149</v>
       </c>
@@ -5483,7 +5515,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="113" spans="1:3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>147</v>
       </c>
@@ -5494,7 +5526,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="114" spans="1:3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>148</v>
       </c>
@@ -5505,9 +5537,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="115" spans="1:3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>6</v>
+        <v>442</v>
       </c>
       <c r="B115" t="s">
         <v>345</v>
@@ -5516,7 +5548,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="116" spans="1:3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>349</v>
       </c>
@@ -5527,7 +5559,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="117" spans="1:3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>14</v>
       </c>
@@ -5538,7 +5570,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="118" spans="1:3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>359</v>
       </c>
@@ -5549,7 +5581,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="119" spans="1:3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>354</v>
       </c>
@@ -5560,7 +5592,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="120" spans="1:3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>155</v>
       </c>
@@ -5571,7 +5603,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="121" spans="1:3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>124</v>
       </c>
@@ -5582,7 +5614,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="122" spans="1:3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>12</v>
       </c>
@@ -5593,7 +5625,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="123" spans="1:3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>119</v>
       </c>
@@ -5604,7 +5636,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="124" spans="1:3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>143</v>
       </c>
@@ -5615,9 +5647,9 @@
         <v>127</v>
       </c>
     </row>
-    <row r="125" spans="1:3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>135</v>
+        <v>441</v>
       </c>
       <c r="B125" t="s">
         <v>345</v>
@@ -5626,9 +5658,9 @@
         <v>129</v>
       </c>
     </row>
-    <row r="126" spans="1:3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>181</v>
+        <v>440</v>
       </c>
       <c r="B126" t="s">
         <v>345</v>
@@ -5637,7 +5669,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="127" spans="1:3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>183</v>
       </c>
@@ -5648,9 +5680,9 @@
         <v>131</v>
       </c>
     </row>
-    <row r="128" spans="1:3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>167</v>
+        <v>445</v>
       </c>
       <c r="B128" t="s">
         <v>345</v>
@@ -5659,7 +5691,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>330</v>
       </c>
@@ -5670,7 +5702,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>353</v>
       </c>
@@ -5681,7 +5713,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>370</v>
       </c>
@@ -5692,7 +5724,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>226</v>
       </c>
@@ -5703,7 +5735,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="133" spans="1:5">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>240</v>
       </c>
@@ -5714,7 +5746,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="134" spans="1:5">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>232</v>
       </c>
@@ -5726,7 +5758,7 @@
       </c>
       <c r="E134" s="1"/>
     </row>
-    <row r="135" spans="1:5">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>256</v>
       </c>
@@ -5737,7 +5769,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="136" spans="1:5">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>360</v>
       </c>
@@ -5748,9 +5780,9 @@
         <v>140</v>
       </c>
     </row>
-    <row r="137" spans="1:5">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>179</v>
+        <v>439</v>
       </c>
       <c r="B137" t="s">
         <v>345</v>
@@ -5759,7 +5791,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="138" spans="1:5">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>369</v>
       </c>
@@ -5770,7 +5802,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="139" spans="1:5">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>222</v>
       </c>
@@ -5781,7 +5813,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="140" spans="1:5">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>367</v>
       </c>
@@ -5792,9 +5824,9 @@
         <v>144</v>
       </c>
     </row>
-    <row r="141" spans="1:5">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>20</v>
+        <v>438</v>
       </c>
       <c r="B141" t="s">
         <v>345</v>
@@ -5803,7 +5835,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="142" spans="1:5">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>333</v>
       </c>
@@ -5814,7 +5846,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="143" spans="1:5">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>437</v>
       </c>
@@ -5825,7 +5857,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="144" spans="1:5">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>104</v>
       </c>
@@ -5836,7 +5868,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="145" spans="1:3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>107</v>
       </c>
@@ -5847,7 +5879,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="146" spans="1:3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>161</v>
       </c>
@@ -5858,7 +5890,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="147" spans="1:3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>93</v>
       </c>
@@ -5869,7 +5901,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="148" spans="1:3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>351</v>
       </c>
@@ -5880,7 +5912,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="149" spans="1:3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>94</v>
       </c>
@@ -5891,7 +5923,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="150" spans="1:3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>95</v>
       </c>
@@ -5902,7 +5934,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="151" spans="1:3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>350</v>
       </c>
@@ -5913,7 +5945,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="152" spans="1:3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>91</v>
       </c>
@@ -5924,7 +5956,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="153" spans="1:3">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>86</v>
       </c>
@@ -5935,7 +5967,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="154" spans="1:3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>199</v>
       </c>
@@ -5946,7 +5978,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="155" spans="1:3">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>213</v>
       </c>
@@ -5957,7 +5989,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="156" spans="1:3">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>249</v>
       </c>
@@ -5968,7 +6000,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="157" spans="1:3">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>243</v>
       </c>
@@ -5979,7 +6011,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="158" spans="1:3">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>110</v>
       </c>
@@ -5990,7 +6022,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="159" spans="1:3">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>75</v>
       </c>
@@ -6001,7 +6033,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="160" spans="1:3">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>77</v>
       </c>
@@ -6027,16 +6059,16 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="43" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>340</v>
       </c>
@@ -6050,7 +6082,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>368</v>
       </c>
@@ -6070,7 +6102,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -6090,7 +6122,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -6110,7 +6142,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>173</v>
       </c>
@@ -6130,7 +6162,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>355</v>
       </c>
@@ -6150,7 +6182,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>356</v>
       </c>
@@ -6170,7 +6202,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>137</v>
       </c>
@@ -6190,7 +6222,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>149</v>
       </c>
@@ -6210,7 +6242,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>147</v>
       </c>
@@ -6230,7 +6262,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>148</v>
       </c>
@@ -6250,7 +6282,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -6270,7 +6302,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>349</v>
       </c>
@@ -6290,7 +6322,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -6310,7 +6342,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>359</v>
       </c>
@@ -6330,7 +6362,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>354</v>
       </c>
@@ -6350,7 +6382,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>155</v>
       </c>
@@ -6370,7 +6402,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>124</v>
       </c>
@@ -6390,7 +6422,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -6410,7 +6442,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>119</v>
       </c>
@@ -6430,7 +6462,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>143</v>
       </c>
@@ -6450,7 +6482,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>135</v>
       </c>
@@ -6470,7 +6502,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>181</v>
       </c>
@@ -6490,7 +6522,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>183</v>
       </c>
@@ -6510,7 +6542,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>167</v>
       </c>
@@ -6530,7 +6562,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>330</v>
       </c>
@@ -6550,7 +6582,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>353</v>
       </c>
@@ -6570,7 +6602,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>370</v>
       </c>
@@ -6590,7 +6622,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>226</v>
       </c>
@@ -6610,7 +6642,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>240</v>
       </c>
@@ -6630,7 +6662,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>232</v>
       </c>
@@ -6650,7 +6682,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>256</v>
       </c>
@@ -6670,7 +6702,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>360</v>
       </c>
@@ -6690,7 +6722,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>179</v>
       </c>
@@ -6710,7 +6742,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>369</v>
       </c>
@@ -6730,7 +6762,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>222</v>
       </c>
@@ -6750,7 +6782,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>367</v>
       </c>
@@ -6770,7 +6802,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>20</v>
       </c>
@@ -6790,7 +6822,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>333</v>
       </c>

</xml_diff>